<commit_message>
completed html tags for sources
</commit_message>
<xml_diff>
--- a/sources/sources.xlsx
+++ b/sources/sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochen\MAI_NLP_PROJECT\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\MAI_NLP_PROJECT\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B8A659-E724-41CF-9121-C64818FD0A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F0F7F5-826E-4ED0-A256-A401176AD909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="21480" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>html box around</t>
   </si>
@@ -118,6 +118,84 @@
   </si>
   <si>
     <t>https://www.smeg.de/sda-kaffeemaschinen/gesamt</t>
+  </si>
+  <si>
+    <t>&lt;div class="dig-pub--text"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href&gt;</t>
+  </si>
+  <si>
+    <t>NOTIZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Together with water boilers, all named "aqua -" </t>
+  </si>
+  <si>
+    <t>&lt;ul class="p-pc05v2__cards p-pc05v2__cards--equalize-inner-height p-pc05v2__cards--portrait-view p-pc05v2--list-view-xs" &gt;</t>
+  </si>
+  <si>
+    <t>&lt;a class="p-pc05v2__card-view-product-link" href&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a class="p-p90__banner p-p90__banner--support" href&gt;</t>
+  </si>
+  <si>
+    <t>&lt;section class="p-st14-manuals-documentation p-prx-data-present p-st14-new-design" data-comp-short-title="Bedienungsanleitung" data-comp-id="st14ManualsDocumentation"&gt;</t>
+  </si>
+  <si>
+    <t>multiple links for multiple languages, need to scrape all</t>
+  </si>
+  <si>
+    <t>&lt;a data-tags="-coffe-makers" href&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="" target="_blank"&gt;</t>
+  </si>
+  <si>
+    <t>bullshit tag without any class links to pdf, maybe check hyperlinks for regex</t>
+  </si>
+  <si>
+    <t>&lt;a class="is-full-area ng-star-inserted" href="" target="_self"&gt;</t>
+  </si>
+  <si>
+    <t>regex in first href for "kaffee"</t>
+  </si>
+  <si>
+    <t>&lt;a class="c__link ng-star-inserted" href="" target="_self"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a id="pagelayout_0_pagetype_0_pagecontent_0_repProducts_hplProduct_0" data-productteaser="link" href=""&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a id="pagelayout_0_pagetype_0_pagecontent_0_tabcontent_0_repManuals_repManualLanguages_0_hplManual_0" href=""&gt;</t>
+  </si>
+  <si>
+    <t>pdf for manual has class 0_hplManual_0, for short manual same with a leading 1</t>
+  </si>
+  <si>
+    <t>&lt;a href="" class="plp-product"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="" class="tech-specs-documents__item-link"&gt;</t>
+  </si>
+  <si>
+    <t>pdf tohether with datasheet, need to exclude "productinformation" from link</t>
+  </si>
+  <si>
+    <t>abfall</t>
+  </si>
+  <si>
+    <t>https://www.illy.com/de-de/kaffeemaschinen/kaffeemaschinen-iperespresso-kapseln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    </t>
+  </si>
+  <si>
+    <t>&lt;div class="product-card__img-item js-product-card-img-item"&gt;&lt;a href&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a class="product-manuals__txt-link" href=""&gt;</t>
   </si>
 </sst>
 </file>
@@ -455,27 +533,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="84.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="40.5546875" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" customWidth="1"/>
-    <col min="9" max="9" width="42.88671875" customWidth="1"/>
-    <col min="10" max="10" width="37.109375" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" customWidth="1"/>
+    <col min="9" max="9" width="42.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="87.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -506,12 +585,15 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -539,19 +621,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
@@ -570,65 +661,155 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{1754A5E2-EB6E-498A-A1A6-6EEBAFAF8B62}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{7D7DB4A4-C0AC-46B1-8477-605DF24474D8}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{C9E79F04-AB0B-46BC-8393-989096B0B789}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{E290F130-CB86-469A-A91C-84B06675D54D}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{20F7C822-0728-45CF-8026-200B3DFBF2FD}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{08E5ACAD-2643-4AB8-8DDE-5177E8D1D9EC}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{88847647-CC77-4E89-9BEF-7F89980E10D3}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{8AB2D635-4CD4-4D1C-AF49-56B99FA66310}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{F6B0DF06-8102-4CBD-A984-8B36DFBFBEDB}"/>
+    <hyperlink ref="B4" r:id="rId10" xr:uid="{0D064F0A-09B0-4A16-9CCB-22B78733ED7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
initial commit for scraper
</commit_message>
<xml_diff>
--- a/sources/sources.xlsx
+++ b/sources/sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\MAI_NLP_PROJECT\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochen\MAI_NLP_PROJECT\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F0F7F5-826E-4ED0-A256-A401176AD909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C21F62-1A61-47B3-89FF-C7159808B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="21480" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -536,25 +536,25 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="91.42578125" customWidth="1"/>
+    <col min="2" max="2" width="91.44140625" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="87.85546875" customWidth="1"/>
+    <col min="6" max="6" width="40.5546875" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" customWidth="1"/>
+    <col min="8" max="8" width="35.5546875" customWidth="1"/>
+    <col min="9" max="9" width="42.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="87.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -589,7 +589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -621,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -638,7 +638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -661,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -684,7 +684,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -701,7 +701,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -721,7 +721,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -738,7 +738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -752,7 +752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -769,25 +769,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
basically its possible to scrape all manuals from from delonghi
</commit_message>
<xml_diff>
--- a/sources/sources.xlsx
+++ b/sources/sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochen\MAI_NLP_PROJECT\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C21F62-1A61-47B3-89FF-C7159808B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74817D7-59EC-4446-9870-49ED8550042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>html box around</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>&lt;a class="product-manuals__txt-link" href=""&gt;</t>
+  </si>
+  <si>
+    <t>dln-instruction-manuals__mainSubtitle für name der maschine</t>
   </si>
 </sst>
 </file>
@@ -535,9 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -620,6 +621,9 @@
       <c r="J2" t="s">
         <v>6</v>
       </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -812,5 +816,6 @@
     <hyperlink ref="B4" r:id="rId10" xr:uid="{0D064F0A-09B0-4A16-9CCB-22B78733ED7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
braun and miele added
</commit_message>
<xml_diff>
--- a/sources/sources.xlsx
+++ b/sources/sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochen\MAI_NLP_PROJECT\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmi\MAI_NLP_PROJECT\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74817D7-59EC-4446-9870-49ED8550042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D60735E-3048-41D2-A357-64E0E1297327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>html box around</t>
   </si>
@@ -199,6 +199,42 @@
   </si>
   <si>
     <t>dln-instruction-manuals__mainSubtitle für name der maschine</t>
+  </si>
+  <si>
+    <t>Miele</t>
+  </si>
+  <si>
+    <t>https://www.miele.de/haushalt/produktauswahl-kaffeevollautomaten-2513.htm</t>
+  </si>
+  <si>
+    <t>Braun</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/produkte/fruehstueck/kaffeemaschinen/c/coffee_machines?q=%3Arelevance%3Acategory_cluster_coffee_makers%3AModerne%2BKaffeemaschine%3Acategory_cluster_coffee_makers%3AStandard-Kaffeemaschine</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/aromaster-kaffeemaschinen/c/aromaster_coffee_machines</t>
+  </si>
+  <si>
+    <t>bedienungsanleitungen -&gt;</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/puraroma-7/c/puraroma_7</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/id-fruehstuecksserie-kaffeemaschinen/c/id_breakfast_collection_coffee_machines</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/purease-kaffeemaschinen/c/purease_coffee_machines</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/cafehouse-coffee-machines/c/cafehouse_coffee_machines</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/multiserve-kaffeemaschine/c/multiserve_coffee_machines</t>
+  </si>
+  <si>
+    <t>https://www.braunhousehold.com/de-de/manuals/produkte/fruehstueck/kaffeemaschinen/breakfast-1-collection-coffee-machines/c/breakfast_1_collection_coffee_machines</t>
   </si>
 </sst>
 </file>
@@ -251,10 +287,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -536,26 +573,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B11:B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="91.44140625" customWidth="1"/>
+    <col min="2" max="2" width="91.453125" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="4" max="4" width="39.90625" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="40.5546875" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" customWidth="1"/>
-    <col min="9" max="9" width="42.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="87.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40.54296875" customWidth="1"/>
+    <col min="7" max="7" width="43.36328125" customWidth="1"/>
+    <col min="8" max="8" width="35.54296875" customWidth="1"/>
+    <col min="9" max="9" width="42.90625" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="11" max="11" width="87.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -590,7 +629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -625,7 +664,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -642,7 +681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -665,7 +704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -688,7 +727,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -705,7 +744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -725,7 +764,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -742,64 +781,111 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="B11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="C14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C22" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -810,12 +896,13 @@
     <hyperlink ref="B6" r:id="rId4" xr:uid="{E290F130-CB86-469A-A91C-84B06675D54D}"/>
     <hyperlink ref="B7" r:id="rId5" xr:uid="{20F7C822-0728-45CF-8026-200B3DFBF2FD}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{08E5ACAD-2643-4AB8-8DDE-5177E8D1D9EC}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{88847647-CC77-4E89-9BEF-7F89980E10D3}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{8AB2D635-4CD4-4D1C-AF49-56B99FA66310}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{F6B0DF06-8102-4CBD-A984-8B36DFBFBEDB}"/>
+    <hyperlink ref="B23" r:id="rId7" xr:uid="{88847647-CC77-4E89-9BEF-7F89980E10D3}"/>
+    <hyperlink ref="B24" r:id="rId8" xr:uid="{8AB2D635-4CD4-4D1C-AF49-56B99FA66310}"/>
+    <hyperlink ref="B22" r:id="rId9" xr:uid="{F6B0DF06-8102-4CBD-A984-8B36DFBFBEDB}"/>
     <hyperlink ref="B4" r:id="rId10" xr:uid="{0D064F0A-09B0-4A16-9CCB-22B78733ED7B}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{8BF04C6C-BA52-49F5-8D69-4A7667683A0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>